<commit_message>
small change in benchmarks excel document
</commit_message>
<xml_diff>
--- a/RobProg/measurements.xlsx
+++ b/RobProg/measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git_projects\software-engineering-f22\RobProg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E64800-52F3-49D4-A86A-6015F91F50DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3845522D-CD32-4338-95B8-981C5914A378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -233,7 +233,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Capability of Magnet</a:t>
+              <a:t> Capability of the Electromagnet</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -317,8 +317,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.17640791776027998"/>
-                  <c:y val="-0.22690616797900262"/>
+                  <c:x val="0.21807458442694663"/>
+                  <c:y val="-0.17135061242344707"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -771,7 +771,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Capability of Magnet</a:t>
+              <a:t> Capability of the Electromagnet</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -855,8 +855,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.15542519685039369"/>
-                  <c:y val="-0.17225503062117237"/>
+                  <c:x val="0.20264741907261594"/>
+                  <c:y val="-0.10554899387576552"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1135,6 +1135,7 @@
         <c:axId val="473080975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3870,8 +3871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>